<commit_message>
Automatische test-sync: 2025-08-13 19:48:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-08-13.xlsx
+++ b/logs/mail_log_2025-08-13.xlsx
@@ -623,7 +623,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J2"/>
+  <dimension ref="A1:J3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -735,8 +735,60 @@
         </is>
       </c>
     </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Demo inplannen</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>klantenservice@testbedrijf123.nl</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Kun je vrijdag om 11:00 een demo inplannen bij Van Dijk?</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>Intern verzoek / Actie voor medewerker</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>Bedankt, we hebben dit doorgestuurd naar planning@testbedrijf123.nl.</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>2025-08-13 19:48:41</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2">
+  <conditionalFormatting sqref="D2:D3">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -756,7 +808,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2">
+  <conditionalFormatting sqref="G2:G3">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -764,17 +816,17 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2">
+  <conditionalFormatting sqref="H2:H3">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2">
+  <conditionalFormatting sqref="I2:I3">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2">
+  <conditionalFormatting sqref="J2:J3">
     <cfRule type="cellIs" priority="11" operator="equal" dxfId="7">
       <formula>"Ja"</formula>
     </cfRule>
@@ -816,7 +868,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Automatische test-sync: 2025-08-13 20:01:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-08-13.xlsx
+++ b/logs/mail_log_2025-08-13.xlsx
@@ -623,7 +623,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J3"/>
+  <dimension ref="A1:J4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -787,8 +787,60 @@
         </is>
       </c>
     </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Demo inplannen</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>klantenservice@testbedrijf123.nl</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Kun je vrijdag om 11:00 een demo inplannen bij Van Dijk?</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>Intern verzoek / Actie voor medewerker</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>Bedankt, we hebben dit doorgestuurd naar planning@testbedrijf123.nl.</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>2025-08-13 20:01:43</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D3">
+  <conditionalFormatting sqref="D2:D4">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -808,7 +860,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G3">
+  <conditionalFormatting sqref="G2:G4">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -816,17 +868,17 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H3">
+  <conditionalFormatting sqref="H2:H4">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I3">
+  <conditionalFormatting sqref="I2:I4">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J3">
+  <conditionalFormatting sqref="J2:J4">
     <cfRule type="cellIs" priority="11" operator="equal" dxfId="7">
       <formula>"Ja"</formula>
     </cfRule>
@@ -868,7 +920,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Automatische test-sync: 2025-08-13 20:15:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-08-13.xlsx
+++ b/logs/mail_log_2025-08-13.xlsx
@@ -623,7 +623,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J4"/>
+  <dimension ref="A1:J5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -839,8 +839,60 @@
         </is>
       </c>
     </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Demo inplannen</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>klantenservice@testbedrijf123.nl</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Kun je vrijdag om 11:00 een demo inplannen bij Van Dijk?</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>Intern verzoek / Actie voor medewerker</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>Bedankt, we hebben dit doorgestuurd naar planning@testbedrijf123.nl.</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>2025-08-13 20:15:02</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="J5" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D4">
+  <conditionalFormatting sqref="D2:D5">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -860,7 +912,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G4">
+  <conditionalFormatting sqref="G2:G5">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -868,17 +920,17 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H4">
+  <conditionalFormatting sqref="H2:H5">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I4">
+  <conditionalFormatting sqref="I2:I5">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J4">
+  <conditionalFormatting sqref="J2:J5">
     <cfRule type="cellIs" priority="11" operator="equal" dxfId="7">
       <formula>"Ja"</formula>
     </cfRule>
@@ -920,7 +972,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Automatische test-sync: 2025-08-13 20:57:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-08-13.xlsx
+++ b/logs/mail_log_2025-08-13.xlsx
@@ -623,7 +623,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J5"/>
+  <dimension ref="A1:J8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -891,8 +891,164 @@
         </is>
       </c>
     </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Demo inplannen</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>klantenservice@testbedrijf123.nl</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Kun je vrijdag om 11:00 een demo inplannen bij Van Dijk?</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>Intern verzoek / Actie voor medewerker</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>Bedankt, we hebben dit doorgestuurd naar planning@testbedrijf123.nl.</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>2025-08-13 20:57:38</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="J6" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Demo inplannen</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>klantenservice@testbedrijf123.nl</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>Kun je vrijdag om 11:00 een demo inplannen bij Van Dijk?</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>Intern verzoek / Actie voor medewerker</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>Bedankt, we hebben dit doorgestuurd naar planning@testbedrijf123.nl.</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>2025-08-13 20:57:40</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="J7" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Demo inplannen</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>klantenservice@testbedrijf123.nl</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>Kun je vrijdag om 11:00 een demo inplannen bij Van Dijk?</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>Intern verzoek / Actie voor medewerker</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>Bedankt, we hebben dit doorgestuurd naar planning@testbedrijf123.nl.</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>2025-08-13 20:57:41</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="I8" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="J8" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D5">
+  <conditionalFormatting sqref="D2:D8">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -912,7 +1068,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G5">
+  <conditionalFormatting sqref="G2:G8">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -920,17 +1076,17 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H5">
+  <conditionalFormatting sqref="H2:H8">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I5">
+  <conditionalFormatting sqref="I2:I8">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J5">
+  <conditionalFormatting sqref="J2:J8">
     <cfRule type="cellIs" priority="11" operator="equal" dxfId="7">
       <formula>"Ja"</formula>
     </cfRule>
@@ -972,7 +1128,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>4</v>
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Automatische test-sync: 2025-08-13 20:58:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-08-13.xlsx
+++ b/logs/mail_log_2025-08-13.xlsx
@@ -623,7 +623,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J8"/>
+  <dimension ref="A1:J9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1047,8 +1047,60 @@
         </is>
       </c>
     </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Demo inplannen</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>klantenservice@testbedrijf123.nl</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>Kun je vrijdag om 11:00 een demo inplannen bij Van Dijk?</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>Intern verzoek / Actie voor medewerker</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>Bedankt, we hebben dit doorgestuurd naar planning@testbedrijf123.nl.</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>2025-08-13 20:58:14</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="I9" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="J9" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D8">
+  <conditionalFormatting sqref="D2:D9">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -1068,7 +1120,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G8">
+  <conditionalFormatting sqref="G2:G9">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1076,17 +1128,17 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H8">
+  <conditionalFormatting sqref="H2:H9">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I8">
+  <conditionalFormatting sqref="I2:I9">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J8">
+  <conditionalFormatting sqref="J2:J9">
     <cfRule type="cellIs" priority="11" operator="equal" dxfId="7">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1128,7 +1180,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Automatische test-sync: 2025-08-13 21:09:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-08-13.xlsx
+++ b/logs/mail_log_2025-08-13.xlsx
@@ -623,7 +623,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J9"/>
+  <dimension ref="A1:J10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1099,8 +1099,60 @@
         </is>
       </c>
     </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Demo inplannen</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>klantenservice@testbedrijf123.nl</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>Kun je vrijdag om 11:00 een demo inplannen bij Van Dijk?</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>Intern verzoek / Actie voor medewerker</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>Bedankt, we hebben dit doorgestuurd naar planning@testbedrijf123.nl.</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>2025-08-13 21:09:38</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="I10" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="J10" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D9">
+  <conditionalFormatting sqref="D2:D10">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -1120,7 +1172,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G9">
+  <conditionalFormatting sqref="G2:G10">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1128,17 +1180,17 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H9">
+  <conditionalFormatting sqref="H2:H10">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I9">
+  <conditionalFormatting sqref="I2:I10">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J9">
+  <conditionalFormatting sqref="J2:J10">
     <cfRule type="cellIs" priority="11" operator="equal" dxfId="7">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1180,7 +1232,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Automatische test-sync: 2025-08-13 21:28:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-08-13.xlsx
+++ b/logs/mail_log_2025-08-13.xlsx
@@ -623,7 +623,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J10"/>
+  <dimension ref="A1:J11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1151,8 +1151,60 @@
         </is>
       </c>
     </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Demo inplannen</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>klantenservice@testbedrijf123.nl</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>Kun je vrijdag om 11:00 een demo inplannen bij Van Dijk?</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>Intern verzoek / Actie voor medewerker</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>Bedankt, we hebben dit doorgestuurd naar planning@testbedrijf123.nl.</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>2025-08-13 21:28:22</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="I11" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="J11" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D10">
+  <conditionalFormatting sqref="D2:D11">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -1172,7 +1224,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G10">
+  <conditionalFormatting sqref="G2:G11">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1180,17 +1232,17 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H10">
+  <conditionalFormatting sqref="H2:H11">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I10">
+  <conditionalFormatting sqref="I2:I11">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J10">
+  <conditionalFormatting sqref="J2:J11">
     <cfRule type="cellIs" priority="11" operator="equal" dxfId="7">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1232,7 +1284,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Automatische test-sync: 2025-08-13 21:44:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-08-13.xlsx
+++ b/logs/mail_log_2025-08-13.xlsx
@@ -623,7 +623,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J11"/>
+  <dimension ref="A1:J12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1203,8 +1203,60 @@
         </is>
       </c>
     </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>Demo inplannen</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>klantenservice@testbedrijf123.nl</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>Kun je vrijdag om 11:00 een demo inplannen bij Van Dijk?</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>Intern verzoek / Actie voor medewerker</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>Bedankt, we hebben dit doorgestuurd naar planning@testbedrijf123.nl.</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>2025-08-13 21:44:48</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="I12" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="J12" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D11">
+  <conditionalFormatting sqref="D2:D12">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -1224,7 +1276,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G11">
+  <conditionalFormatting sqref="G2:G12">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1232,17 +1284,17 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H11">
+  <conditionalFormatting sqref="H2:H12">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I11">
+  <conditionalFormatting sqref="I2:I12">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J11">
+  <conditionalFormatting sqref="J2:J12">
     <cfRule type="cellIs" priority="11" operator="equal" dxfId="7">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1284,7 +1336,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Automatische test-sync: 2025-08-13 21:45:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-08-13.xlsx
+++ b/logs/mail_log_2025-08-13.xlsx
@@ -623,7 +623,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J12"/>
+  <dimension ref="A1:J13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1255,8 +1255,60 @@
         </is>
       </c>
     </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>Demo inplannen</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>klantenservice@testbedrijf123.nl</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>Kun je vrijdag om 11:00 een demo inplannen bij Van Dijk?</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>Intern verzoek / Actie voor medewerker</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>Bedankt, we hebben dit doorgestuurd naar planning@testbedrijf123.nl.</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>2025-08-13 21:45:14</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="I13" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="J13" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D12">
+  <conditionalFormatting sqref="D2:D13">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -1276,7 +1328,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G12">
+  <conditionalFormatting sqref="G2:G13">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1284,17 +1336,17 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H12">
+  <conditionalFormatting sqref="H2:H13">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I12">
+  <conditionalFormatting sqref="I2:I13">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J12">
+  <conditionalFormatting sqref="J2:J13">
     <cfRule type="cellIs" priority="11" operator="equal" dxfId="7">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1336,7 +1388,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Automatische test-sync: 2025-08-13 21:46:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-08-13.xlsx
+++ b/logs/mail_log_2025-08-13.xlsx
@@ -623,7 +623,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J13"/>
+  <dimension ref="A1:J17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1307,8 +1307,230 @@
         </is>
       </c>
     </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>Re: Demo inplannen</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>admin@testbedrijf123.nl</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>Bedankt, we hebben dit doorgestuurd naar planning@testbedrijf123.nl.</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>Intern verzoek / Actie voor medewerker</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>Bedankt, we hebben dit doorgestuurd naar planning@testbedrijf123.nl.</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>2025-08-13 21:46:07</t>
+        </is>
+      </c>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="H14" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="I14" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="J14" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>[Fallback] Handmatige opvolging: Demo inplannen</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>admin@testbedrijf123.nl</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>Beste collega,
+Onderstaande e-mail kon niet automatisch worden beantwoord door het AI-systeem. Wil je deze even opvolgen?
+📩 Originele afzender: klantenservice@testbedrijf123.nl
+📝 Onderwerp: Demo inplannen
+🔎 Reden: Interne afzender
+━━━━━━━━━━━━━━━━━━━━━━━━━━━
+✉️ Bericht:
+Kun je vrijdag om 11:00 een demo inplannen bij Van Dijk?
+━━━━━━━━━━━━━━━━━━━━━━━━━━━
+Met vriendelijke groet,
+MailMind Automatische Assistent
+—
+[Bedrijfsnaam]
+klantenservice@bedrijf.nl
+www.bedrijf.nl</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>Intern verzoek / Actie voor medewerker</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>Bedankt, we hebben dit doorgestuurd naar planning@testbedrijf123.nl.</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>2025-08-13 21:46:08</t>
+        </is>
+      </c>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="H15" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="I15" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="J15" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>Demo inplannen</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>klantenservice@testbedrijf123.nl</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>Kun je vrijdag om 11:00 een demo inplannen bij Van Dijk?</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>Intern verzoek / Actie voor medewerker</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>Bedankt, we hebben dit doorgestuurd naar planning@testbedrijf123.nl.</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>2025-08-13 21:46:09</t>
+        </is>
+      </c>
+      <c r="G16" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="H16" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="I16" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="J16" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>Demo inplannen</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>klantenservice@testbedrijf123.nl</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>Kun je vrijdag om 11:00 een demo inplannen bij Van Dijk?</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>Intern verzoek / Actie voor medewerker</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>Bedankt, we hebben dit doorgestuurd naar planning@testbedrijf123.nl.</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>2025-08-13 21:46:35</t>
+        </is>
+      </c>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="H17" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="I17" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="J17" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D13">
+  <conditionalFormatting sqref="D2:D17">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -1328,7 +1550,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G13">
+  <conditionalFormatting sqref="G2:G17">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1336,17 +1558,17 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H13">
+  <conditionalFormatting sqref="H2:H17">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I13">
+  <conditionalFormatting sqref="I2:I17">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J13">
+  <conditionalFormatting sqref="J2:J17">
     <cfRule type="cellIs" priority="11" operator="equal" dxfId="7">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1388,7 +1610,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>12</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Automatische test-sync: 2025-08-13 21:47:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-08-13.xlsx
+++ b/logs/mail_log_2025-08-13.xlsx
@@ -623,7 +623,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J17"/>
+  <dimension ref="A1:J18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1529,8 +1529,60 @@
         </is>
       </c>
     </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>Demo inplannen</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>klantenservice@testbedrijf123.nl</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>Kun je vrijdag om 11:00 een demo inplannen bij Van Dijk?</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>Intern verzoek / Actie voor medewerker</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>Bedankt, we hebben dit doorgestuurd naar planning@testbedrijf123.nl.</t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>2025-08-13 21:47:40</t>
+        </is>
+      </c>
+      <c r="G18" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="H18" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="I18" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="J18" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D17">
+  <conditionalFormatting sqref="D2:D18">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -1550,7 +1602,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G17">
+  <conditionalFormatting sqref="G2:G18">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1558,17 +1610,17 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H17">
+  <conditionalFormatting sqref="H2:H18">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I17">
+  <conditionalFormatting sqref="I2:I18">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J17">
+  <conditionalFormatting sqref="J2:J18">
     <cfRule type="cellIs" priority="11" operator="equal" dxfId="7">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1610,7 +1662,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Automatische test-sync: 2025-08-13 21:55:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-08-13.xlsx
+++ b/logs/mail_log_2025-08-13.xlsx
@@ -623,7 +623,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J18"/>
+  <dimension ref="A1:J20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1581,8 +1581,126 @@
         </is>
       </c>
     </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>[Fallback] Handmatige opvolging: Demo inplannen</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>admin@testbedrijf123.nl</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>Beste collega,
+Onderstaande e-mail kon niet automatisch worden beantwoord door het AI-systeem. Wil je deze even opvolgen?
+📩 Originele afzender: klantenservice@testbedrijf123.nl
+📝 Onderwerp: Demo inplannen
+🔎 Reden: Interne afzender
+━━━━━━━━━━━━━━━━━━━━━━━━━━━
+✉️ Bericht:
+Kun je vrijdag om 11:00 een demo inplannen bij Van Dijk?
+━━━━━━━━━━━━━━━━━━━━━━━━━━━
+Met vriendelijke groet,
+MailMind Automatische Assistent
+—
+[Bedrijfsnaam]
+klantenservice@bedrijf.nl
+www.bedrijf.nl</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>Intern verzoek / Actie voor medewerker</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>Bedankt, we hebben dit doorgestuurd naar planning@testbedrijf123.nl.</t>
+        </is>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>2025-08-13 21:55:30</t>
+        </is>
+      </c>
+      <c r="G19" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="H19" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="I19" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="J19" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>Demo inplannen</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>klantenservice@testbedrijf123.nl</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>Kun je vrijdag om 11:00 een demo inplannen bij Van Dijk?</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>Intern verzoek / Actie voor medewerker</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>Bedankt, we hebben dit doorgestuurd naar planning@testbedrijf123.nl.</t>
+        </is>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>2025-08-13 21:55:31</t>
+        </is>
+      </c>
+      <c r="G20" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="H20" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="I20" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="J20" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D18">
+  <conditionalFormatting sqref="D2:D20">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -1602,7 +1720,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G18">
+  <conditionalFormatting sqref="G2:G20">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1610,17 +1728,17 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H18">
+  <conditionalFormatting sqref="H2:H20">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I18">
+  <conditionalFormatting sqref="I2:I20">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J18">
+  <conditionalFormatting sqref="J2:J20">
     <cfRule type="cellIs" priority="11" operator="equal" dxfId="7">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1662,7 +1780,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>17</v>
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Automatische test-sync: 2025-08-13 21:56:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-08-13.xlsx
+++ b/logs/mail_log_2025-08-13.xlsx
@@ -623,7 +623,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J20"/>
+  <dimension ref="A1:J21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1699,8 +1699,60 @@
         </is>
       </c>
     </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>Demo inplannen</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>klantenservice@testbedrijf123.nl</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>Kun je vrijdag om 11:00 een demo inplannen bij Van Dijk?</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>Intern verzoek / Actie voor medewerker</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>Bedankt, we hebben dit doorgestuurd naar planning@testbedrijf123.nl.</t>
+        </is>
+      </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>2025-08-13 21:55:58</t>
+        </is>
+      </c>
+      <c r="G21" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="H21" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="I21" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="J21" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D20">
+  <conditionalFormatting sqref="D2:D21">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -1720,7 +1772,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G20">
+  <conditionalFormatting sqref="G2:G21">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1728,17 +1780,17 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H20">
+  <conditionalFormatting sqref="H2:H21">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I20">
+  <conditionalFormatting sqref="I2:I21">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J20">
+  <conditionalFormatting sqref="J2:J21">
     <cfRule type="cellIs" priority="11" operator="equal" dxfId="7">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1780,7 +1832,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Automatische test-sync: 2025-08-13 22:09:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-08-13.xlsx
+++ b/logs/mail_log_2025-08-13.xlsx
@@ -623,7 +623,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J21"/>
+  <dimension ref="A1:J22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1751,8 +1751,60 @@
         </is>
       </c>
     </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>Demo inplannen</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>klantenservice@testbedrijf123.nl</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>Kun je vrijdag om 11:00 een demo inplannen bij Van Dijk?</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>Intern verzoek / Actie voor medewerker</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>Bedankt, we hebben dit doorgestuurd naar planning@testbedrijf123.nl.</t>
+        </is>
+      </c>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>2025-08-13 22:08:50</t>
+        </is>
+      </c>
+      <c r="G22" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="H22" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="I22" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="J22" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D21">
+  <conditionalFormatting sqref="D2:D22">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -1772,7 +1824,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G21">
+  <conditionalFormatting sqref="G2:G22">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1780,17 +1832,17 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H21">
+  <conditionalFormatting sqref="H2:H22">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I21">
+  <conditionalFormatting sqref="I2:I22">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J21">
+  <conditionalFormatting sqref="J2:J22">
     <cfRule type="cellIs" priority="11" operator="equal" dxfId="7">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1832,7 +1884,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Automatische test-sync: 2025-08-13 22:10:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-08-13.xlsx
+++ b/logs/mail_log_2025-08-13.xlsx
@@ -623,7 +623,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J22"/>
+  <dimension ref="A1:J23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1803,8 +1803,60 @@
         </is>
       </c>
     </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>Demo inplannen</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>klantenservice@testbedrijf123.nl</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>Kun je vrijdag om 11:00 een demo inplannen bij Van Dijk?</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>Intern verzoek / Actie voor medewerker</t>
+        </is>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>Bedankt, we hebben dit doorgestuurd naar planning@testbedrijf123.nl.</t>
+        </is>
+      </c>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>2025-08-13 22:10:01</t>
+        </is>
+      </c>
+      <c r="G23" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="H23" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="I23" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="J23" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D22">
+  <conditionalFormatting sqref="D2:D23">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -1824,7 +1876,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G22">
+  <conditionalFormatting sqref="G2:G23">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1832,17 +1884,17 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H22">
+  <conditionalFormatting sqref="H2:H23">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I22">
+  <conditionalFormatting sqref="I2:I23">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J22">
+  <conditionalFormatting sqref="J2:J23">
     <cfRule type="cellIs" priority="11" operator="equal" dxfId="7">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1884,7 +1936,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Automatische test-sync: 2025-08-13 22:16:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-08-13.xlsx
+++ b/logs/mail_log_2025-08-13.xlsx
@@ -623,7 +623,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J23"/>
+  <dimension ref="A1:J24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1855,8 +1855,60 @@
         </is>
       </c>
     </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>Demo inplannen</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>klantenservice@testbedrijf123.nl</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>Kun je vrijdag om 11:00 een demo inplannen bij Van Dijk?</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>Intern verzoek / Actie voor medewerker</t>
+        </is>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>Bedankt, we hebben dit doorgestuurd naar planning@testbedrijf123.nl.</t>
+        </is>
+      </c>
+      <c r="F24" t="inlineStr">
+        <is>
+          <t>2025-08-13 22:16:16</t>
+        </is>
+      </c>
+      <c r="G24" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="H24" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="I24" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="J24" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D23">
+  <conditionalFormatting sqref="D2:D24">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -1876,7 +1928,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G23">
+  <conditionalFormatting sqref="G2:G24">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1884,17 +1936,17 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H23">
+  <conditionalFormatting sqref="H2:H24">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I23">
+  <conditionalFormatting sqref="I2:I24">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J23">
+  <conditionalFormatting sqref="J2:J24">
     <cfRule type="cellIs" priority="11" operator="equal" dxfId="7">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1936,7 +1988,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Automatische test-sync: 2025-08-13 22:19:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-08-13.xlsx
+++ b/logs/mail_log_2025-08-13.xlsx
@@ -623,7 +623,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J24"/>
+  <dimension ref="A1:J25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1907,8 +1907,60 @@
         </is>
       </c>
     </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>Demo inplannen</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>klantenservice@testbedrijf123.nl</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>Kun je vrijdag om 11:00 een demo inplannen bij Van Dijk?</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>Intern verzoek / Actie voor medewerker</t>
+        </is>
+      </c>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>Bedankt, we hebben dit doorgestuurd naar planning@testbedrijf123.nl.</t>
+        </is>
+      </c>
+      <c r="F25" t="inlineStr">
+        <is>
+          <t>2025-08-13 22:19:22</t>
+        </is>
+      </c>
+      <c r="G25" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="H25" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="I25" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="J25" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D24">
+  <conditionalFormatting sqref="D2:D25">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -1928,7 +1980,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G24">
+  <conditionalFormatting sqref="G2:G25">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1936,17 +1988,17 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H24">
+  <conditionalFormatting sqref="H2:H25">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I24">
+  <conditionalFormatting sqref="I2:I25">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J24">
+  <conditionalFormatting sqref="J2:J25">
     <cfRule type="cellIs" priority="11" operator="equal" dxfId="7">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1988,7 +2040,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Automatische test-sync: 2025-08-13 22:26:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-08-13.xlsx
+++ b/logs/mail_log_2025-08-13.xlsx
@@ -623,7 +623,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J25"/>
+  <dimension ref="A1:J26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1959,8 +1959,60 @@
         </is>
       </c>
     </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>Demo inplannen</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>klantenservice@testbedrijf123.nl</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>Kun je vrijdag om 11:00 een demo inplannen bij Van Dijk?</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>Intern verzoek / Actie voor medewerker</t>
+        </is>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>Bedankt, we hebben dit doorgestuurd naar planning@testbedrijf123.nl.</t>
+        </is>
+      </c>
+      <c r="F26" t="inlineStr">
+        <is>
+          <t>2025-08-13 22:26:49</t>
+        </is>
+      </c>
+      <c r="G26" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="H26" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="I26" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="J26" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D25">
+  <conditionalFormatting sqref="D2:D26">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -1980,7 +2032,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G25">
+  <conditionalFormatting sqref="G2:G26">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1988,17 +2040,17 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H25">
+  <conditionalFormatting sqref="H2:H26">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I25">
+  <conditionalFormatting sqref="I2:I26">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J25">
+  <conditionalFormatting sqref="J2:J26">
     <cfRule type="cellIs" priority="11" operator="equal" dxfId="7">
       <formula>"Ja"</formula>
     </cfRule>
@@ -2040,7 +2092,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Automatische test-sync: 2025-08-13 22:28:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-08-13.xlsx
+++ b/logs/mail_log_2025-08-13.xlsx
@@ -623,7 +623,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J26"/>
+  <dimension ref="A1:J27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2011,8 +2011,60 @@
         </is>
       </c>
     </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>Demo inplannen</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>klantenservice@testbedrijf123.nl</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>Kun je vrijdag om 11:00 een demo inplannen bij Van Dijk?</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>Intern verzoek / Actie voor medewerker</t>
+        </is>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>Bedankt, we hebben dit doorgestuurd naar planning@testbedrijf123.nl.</t>
+        </is>
+      </c>
+      <c r="F27" t="inlineStr">
+        <is>
+          <t>2025-08-13 22:28:12</t>
+        </is>
+      </c>
+      <c r="G27" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="H27" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="I27" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="J27" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D26">
+  <conditionalFormatting sqref="D2:D27">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -2032,7 +2084,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G26">
+  <conditionalFormatting sqref="G2:G27">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -2040,17 +2092,17 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H26">
+  <conditionalFormatting sqref="H2:H27">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I26">
+  <conditionalFormatting sqref="I2:I27">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J26">
+  <conditionalFormatting sqref="J2:J27">
     <cfRule type="cellIs" priority="11" operator="equal" dxfId="7">
       <formula>"Ja"</formula>
     </cfRule>
@@ -2092,7 +2144,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Automatische test-sync: 2025-08-13 22:42:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-08-13.xlsx
+++ b/logs/mail_log_2025-08-13.xlsx
@@ -623,7 +623,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J27"/>
+  <dimension ref="A1:J28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2063,8 +2063,60 @@
         </is>
       </c>
     </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>Demo inplannen</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>klantenservice@testbedrijf123.nl</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>Kun je vrijdag om 11:00 een demo inplannen bij Van Dijk?</t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>Intern verzoek / Actie voor medewerker</t>
+        </is>
+      </c>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>Bedankt, we hebben dit doorgestuurd naar planning@testbedrijf123.nl.</t>
+        </is>
+      </c>
+      <c r="F28" t="inlineStr">
+        <is>
+          <t>2025-08-13 22:42:46</t>
+        </is>
+      </c>
+      <c r="G28" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="H28" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="I28" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="J28" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D27">
+  <conditionalFormatting sqref="D2:D28">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -2084,7 +2136,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G27">
+  <conditionalFormatting sqref="G2:G28">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -2092,17 +2144,17 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H27">
+  <conditionalFormatting sqref="H2:H28">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I27">
+  <conditionalFormatting sqref="I2:I28">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J27">
+  <conditionalFormatting sqref="J2:J28">
     <cfRule type="cellIs" priority="11" operator="equal" dxfId="7">
       <formula>"Ja"</formula>
     </cfRule>
@@ -2144,7 +2196,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Automatische test-sync: 2025-08-13 22:49:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-08-13.xlsx
+++ b/logs/mail_log_2025-08-13.xlsx
@@ -623,7 +623,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J28"/>
+  <dimension ref="A1:J29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2115,8 +2115,60 @@
         </is>
       </c>
     </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>Demo inplannen</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>klantenservice@testbedrijf123.nl</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>Kun je vrijdag om 11:00 een demo inplannen bij Van Dijk?</t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>Intern verzoek / Actie voor medewerker</t>
+        </is>
+      </c>
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>Bedankt, we hebben dit doorgestuurd naar planning@testbedrijf123.nl.</t>
+        </is>
+      </c>
+      <c r="F29" t="inlineStr">
+        <is>
+          <t>2025-08-13 22:49:12</t>
+        </is>
+      </c>
+      <c r="G29" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="H29" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="I29" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="J29" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D28">
+  <conditionalFormatting sqref="D2:D29">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -2136,7 +2188,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G28">
+  <conditionalFormatting sqref="G2:G29">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -2144,17 +2196,17 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H28">
+  <conditionalFormatting sqref="H2:H29">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I28">
+  <conditionalFormatting sqref="I2:I29">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J28">
+  <conditionalFormatting sqref="J2:J29">
     <cfRule type="cellIs" priority="11" operator="equal" dxfId="7">
       <formula>"Ja"</formula>
     </cfRule>
@@ -2196,7 +2248,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Automatische test-sync: 2025-08-13 22:51:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-08-13.xlsx
+++ b/logs/mail_log_2025-08-13.xlsx
@@ -623,7 +623,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J29"/>
+  <dimension ref="A1:J30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2167,8 +2167,60 @@
         </is>
       </c>
     </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>Demo inplannen</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>klantenservice@testbedrijf123.nl</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>Kun je vrijdag om 11:00 een demo inplannen bij Van Dijk?</t>
+        </is>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>Intern verzoek / Actie voor medewerker</t>
+        </is>
+      </c>
+      <c r="E30" t="inlineStr">
+        <is>
+          <t>Bedankt, we hebben dit doorgestuurd naar planning@testbedrijf123.nl.</t>
+        </is>
+      </c>
+      <c r="F30" t="inlineStr">
+        <is>
+          <t>2025-08-13 22:51:45</t>
+        </is>
+      </c>
+      <c r="G30" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="H30" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="I30" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="J30" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D29">
+  <conditionalFormatting sqref="D2:D30">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -2188,7 +2240,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G29">
+  <conditionalFormatting sqref="G2:G30">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -2196,17 +2248,17 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H29">
+  <conditionalFormatting sqref="H2:H30">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I29">
+  <conditionalFormatting sqref="I2:I30">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J29">
+  <conditionalFormatting sqref="J2:J30">
     <cfRule type="cellIs" priority="11" operator="equal" dxfId="7">
       <formula>"Ja"</formula>
     </cfRule>
@@ -2248,7 +2300,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Automatische test-sync: 2025-08-13 22:54:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-08-13.xlsx
+++ b/logs/mail_log_2025-08-13.xlsx
@@ -623,7 +623,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J30"/>
+  <dimension ref="A1:J31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2219,8 +2219,60 @@
         </is>
       </c>
     </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>Demo inplannen</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>klantenservice@testbedrijf123.nl</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>Kun je vrijdag om 11:00 een demo inplannen bij Van Dijk?</t>
+        </is>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>Intern verzoek / Actie voor medewerker</t>
+        </is>
+      </c>
+      <c r="E31" t="inlineStr">
+        <is>
+          <t>Bedankt, we hebben dit doorgestuurd naar planning@testbedrijf123.nl.</t>
+        </is>
+      </c>
+      <c r="F31" t="inlineStr">
+        <is>
+          <t>2025-08-13 22:54:21</t>
+        </is>
+      </c>
+      <c r="G31" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="H31" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="I31" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="J31" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D30">
+  <conditionalFormatting sqref="D2:D31">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -2240,7 +2292,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G30">
+  <conditionalFormatting sqref="G2:G31">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -2248,17 +2300,17 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H30">
+  <conditionalFormatting sqref="H2:H31">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I30">
+  <conditionalFormatting sqref="I2:I31">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J30">
+  <conditionalFormatting sqref="J2:J31">
     <cfRule type="cellIs" priority="11" operator="equal" dxfId="7">
       <formula>"Ja"</formula>
     </cfRule>
@@ -2300,7 +2352,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>